<commit_message>
Final version for today
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="28740" windowHeight="12984"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28740" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,19 +16,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Количество верхней одежды</t>
   </si>
   <si>
     <t>Количество нижней</t>
+  </si>
+  <si>
+    <t>0+0+1</t>
+  </si>
+  <si>
+    <t>0+1+2</t>
+  </si>
+  <si>
+    <t>1+2+3</t>
+  </si>
+  <si>
+    <t>нет</t>
+  </si>
+  <si>
+    <t>Можно ли что то надеть над?</t>
+  </si>
+  <si>
+    <t>Можно ли что то надеть под?</t>
+  </si>
+  <si>
+    <t>Диапазон температур</t>
+  </si>
+  <si>
+    <t>&gt;23</t>
+  </si>
+  <si>
+    <t>Водолазка</t>
+  </si>
+  <si>
+    <t>Футболка</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18-25</t>
+  </si>
+  <si>
+    <t>Кофта</t>
+  </si>
+  <si>
+    <t>нужно</t>
+  </si>
+  <si>
+    <t>только 3 слой</t>
+  </si>
+  <si>
+    <t>да 2-3слой</t>
+  </si>
+  <si>
+    <t>да 2-3 слой</t>
+  </si>
+  <si>
+    <t>от 8 до 18</t>
+  </si>
+  <si>
+    <t>1 слой</t>
+  </si>
+  <si>
+    <t>2 слой</t>
+  </si>
+  <si>
+    <t>3 слой</t>
+  </si>
+  <si>
+    <t>Пальто</t>
+  </si>
+  <si>
+    <t>нужно 2</t>
+  </si>
+  <si>
+    <t>минус 10 до 8</t>
+  </si>
+  <si>
+    <t>Пиджак/Блейзер</t>
+  </si>
+  <si>
+    <t>Домашне</t>
+  </si>
+  <si>
+    <t>Спорт</t>
+  </si>
+  <si>
+    <t>Кэжуал</t>
+  </si>
+  <si>
+    <t>Элегантный</t>
+  </si>
+  <si>
+    <t>Бизнес</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,8 +127,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -63,6 +160,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -76,11 +185,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -382,27 +495,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>30</v>
       </c>
@@ -412,8 +545,26 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>28</v>
       </c>
@@ -423,8 +574,29 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>26</v>
       </c>
@@ -434,8 +606,29 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>24</v>
       </c>
@@ -445,8 +638,26 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>22</v>
       </c>
@@ -457,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>20</v>
       </c>
@@ -468,7 +679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>18</v>
       </c>
@@ -478,8 +689,23 @@
       <c r="C8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>16</v>
       </c>
@@ -489,8 +715,21 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>14</v>
       </c>
@@ -500,8 +739,21 @@
       <c r="C10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -511,8 +763,21 @@
       <c r="C11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -522,8 +787,21 @@
       <c r="C12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -533,8 +811,21 @@
       <c r="C13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
@@ -545,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -555,8 +846,14 @@
       <c r="C15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -567,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -578,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-2</v>
       </c>
@@ -589,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-4</v>
       </c>
@@ -599,8 +896,28 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <f>36 - 23</f>
+        <v>13</v>
+      </c>
+      <c r="J19">
+        <f>36-18</f>
+        <v>18</v>
+      </c>
+      <c r="K19">
+        <f>36-8</f>
+        <v>28</v>
+      </c>
+      <c r="L19">
+        <f>36-8</f>
+        <v>28</v>
+      </c>
+      <c r="M19">
+        <f>36-21</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-6</v>
       </c>
@@ -610,8 +927,27 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <f>36-25</f>
+        <v>11</v>
+      </c>
+      <c r="K20">
+        <f>36-18</f>
+        <v>18</v>
+      </c>
+      <c r="L20">
+        <f>36-18</f>
+        <v>18</v>
+      </c>
+      <c r="M20">
+        <f>36-6</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-8</v>
       </c>
@@ -621,8 +957,28 @@
       <c r="C21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <f>(I19+I20)/2</f>
+        <v>9.5</v>
+      </c>
+      <c r="J21">
+        <f>(J19+J20)/2</f>
+        <v>14.5</v>
+      </c>
+      <c r="K21">
+        <f>(K19+K20)/2</f>
+        <v>23</v>
+      </c>
+      <c r="L21">
+        <f>(L19+L20)/2</f>
+        <v>23</v>
+      </c>
+      <c r="M21">
+        <f>(M19+M20)/2</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-10</v>
       </c>
@@ -633,7 +989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-12</v>
       </c>
@@ -644,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-14</v>
       </c>
@@ -655,7 +1011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-16</v>
       </c>
@@ -666,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-18</v>
       </c>
@@ -677,7 +1033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-20</v>
       </c>
@@ -688,7 +1044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-22</v>
       </c>
@@ -699,7 +1055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-24</v>
       </c>
@@ -710,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-26</v>
       </c>
@@ -721,7 +1077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-28</v>
       </c>
@@ -732,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-30</v>
       </c>
@@ -745,6 +1101,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -754,7 +1111,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -766,7 +1123,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New algorithm with forecast
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Количество верхней одежды</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>openweather:</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>погода в</t>
+  </si>
+  <si>
+    <t>Появился</t>
+  </si>
+  <si>
+    <t>(a-b)/2</t>
   </si>
 </sst>
 </file>
@@ -185,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -194,6 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -495,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +522,7 @@
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.85546875" customWidth="1"/>
@@ -535,7 +551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30</v>
       </c>
@@ -564,7 +580,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>28</v>
       </c>
@@ -596,7 +612,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>26</v>
       </c>
@@ -628,7 +644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>24</v>
       </c>
@@ -679,7 +695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>18</v>
       </c>
@@ -705,7 +721,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16</v>
       </c>
@@ -729,7 +745,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
@@ -777,7 +793,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -801,7 +817,7 @@
       </c>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1032,6 +1048,15 @@
       <c r="C26" s="3">
         <v>2</v>
       </c>
+      <c r="I26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1043,6 +1068,15 @@
       <c r="C27" s="3">
         <v>2</v>
       </c>
+      <c r="I27" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="8">
+        <v>0.625</v>
+      </c>
+      <c r="K27" s="8">
+        <v>0.58333333333333337</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1054,6 +1088,12 @@
       <c r="C28" s="3">
         <v>2</v>
       </c>
+      <c r="J28" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="K28" s="8">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -1087,6 +1127,9 @@
       <c r="C31" s="3">
         <v>2</v>
       </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1097,6 +1140,129 @@
       </c>
       <c r="C32" s="3">
         <v>2</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>14</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <v>2</v>
+      </c>
+      <c r="M42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>15</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>3</v>
+      </c>
+      <c r="L43">
+        <v>2</v>
+      </c>
+      <c r="M43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>16</v>
+      </c>
+      <c r="J44">
+        <v>-1</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <v>2</v>
+      </c>
+      <c r="M44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>17</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
+      <c r="M45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>18</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>19</v>
+      </c>
+      <c r="J47">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start to use Enum
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28740" windowHeight="12990"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="23280" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>Количество верхней одежды</t>
   </si>
@@ -24,15 +25,6 @@
     <t>Количество нижней</t>
   </si>
   <si>
-    <t>0+0+1</t>
-  </si>
-  <si>
-    <t>0+1+2</t>
-  </si>
-  <si>
-    <t>1+2+3</t>
-  </si>
-  <si>
     <t>нет</t>
   </si>
   <si>
@@ -51,15 +43,9 @@
     <t>Водолазка</t>
   </si>
   <si>
-    <t>Футболка</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 18-25</t>
   </si>
   <si>
-    <t>Кофта</t>
-  </si>
-  <si>
     <t>нужно</t>
   </si>
   <si>
@@ -84,18 +70,12 @@
     <t>3 слой</t>
   </si>
   <si>
-    <t>Пальто</t>
-  </si>
-  <si>
     <t>нужно 2</t>
   </si>
   <si>
     <t>минус 10 до 8</t>
   </si>
   <si>
-    <t>Пиджак/Блейзер</t>
-  </si>
-  <si>
     <t>Домашне</t>
   </si>
   <si>
@@ -127,13 +107,79 @@
   </si>
   <si>
     <t>(a-b)/2</t>
+  </si>
+  <si>
+    <t>30-23</t>
+  </si>
+  <si>
+    <t>Пальто/Куртка</t>
+  </si>
+  <si>
+    <t>Кофта/Пиджак/Блейзер</t>
+  </si>
+  <si>
+    <t>от 7 до 17</t>
+  </si>
+  <si>
+    <t>4+1</t>
+  </si>
+  <si>
+    <t>4+2</t>
+  </si>
+  <si>
+    <t>3+1</t>
+  </si>
+  <si>
+    <t>3+2</t>
+  </si>
+  <si>
+    <t>5+2</t>
+  </si>
+  <si>
+    <t>Куртка легкая</t>
+  </si>
+  <si>
+    <t>Футболка/рубашка</t>
+  </si>
+  <si>
+    <t>5+1</t>
+  </si>
+  <si>
+    <t>4+3</t>
+  </si>
+  <si>
+    <t>4+3+1</t>
+  </si>
+  <si>
+    <t>5+3+2</t>
+  </si>
+  <si>
+    <t>3+2+1</t>
+  </si>
+  <si>
+    <t>5+3 + 1</t>
+  </si>
+  <si>
+    <t>5+3+2 +1</t>
+  </si>
+  <si>
+    <t>people bath ac uk</t>
+  </si>
+  <si>
+    <t>air velocity=0</t>
+  </si>
+  <si>
+    <t>humidity 50%</t>
+  </si>
+  <si>
+    <t>tem\clo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +190,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -200,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -210,6 +264,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -514,7 +572,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,9 +580,9 @@
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
     <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -536,19 +594,19 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -561,23 +619,29 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>2</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -590,26 +654,32 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>3</v>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -622,26 +692,32 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>4</v>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -654,26 +730,35 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
       <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
       <c r="K5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>22</v>
       </c>
@@ -683,8 +768,32 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -693,6 +802,18 @@
       </c>
       <c r="C7" s="1">
         <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -705,20 +826,29 @@
       <c r="C8" s="2">
         <v>1</v>
       </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="M8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -731,14 +861,20 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
       <c r="G9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="3"/>
@@ -755,15 +891,21 @@
       <c r="C10" s="2">
         <v>1</v>
       </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
       <c r="G10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="3"/>
@@ -779,16 +921,25 @@
       <c r="C11" s="2">
         <v>1</v>
       </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11">
+        <v>4.5</v>
+      </c>
       <c r="G11">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="7"/>
@@ -803,17 +954,26 @@
       <c r="C12" s="2">
         <v>1</v>
       </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
       <c r="G12">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="5"/>
       <c r="L12" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="M12" s="5"/>
     </row>
@@ -827,21 +987,30 @@
       <c r="C13" s="2">
         <v>1</v>
       </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
       <c r="G13">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="5"/>
       <c r="M13" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -851,8 +1020,20 @@
       <c r="C14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -862,8 +1043,17 @@
       <c r="C15" s="2">
         <v>1</v>
       </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
       <c r="G15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H15">
         <v>23</v>
@@ -878,6 +1068,18 @@
       </c>
       <c r="C16" s="2">
         <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -890,6 +1092,15 @@
       <c r="C17" s="2">
         <v>1</v>
       </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -901,6 +1112,15 @@
       <c r="C18" s="2">
         <v>1</v>
       </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -912,6 +1132,15 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>17</v>
+      </c>
       <c r="I19">
         <f>36 - 23</f>
         <v>13</v>
@@ -943,6 +1172,15 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>18</v>
+      </c>
       <c r="I20">
         <v>6</v>
       </c>
@@ -973,6 +1211,15 @@
       <c r="C21" s="2">
         <v>1</v>
       </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21">
+        <v>11</v>
+      </c>
+      <c r="G21">
+        <v>19</v>
+      </c>
       <c r="I21">
         <f>(I19+I20)/2</f>
         <v>9.5</v>
@@ -1004,6 +1251,15 @@
       <c r="C22" s="3">
         <v>2</v>
       </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22">
+        <v>11</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1049,13 +1305,13 @@
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="J26" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1069,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="J27" s="8">
         <v>0.625</v>
@@ -1190,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="M42" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="9:13" x14ac:dyDescent="0.25">
@@ -1207,7 +1463,7 @@
         <v>2</v>
       </c>
       <c r="M43" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="9:13" x14ac:dyDescent="0.25">
@@ -1224,7 +1480,7 @@
         <v>2</v>
       </c>
       <c r="M44" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="9:13" x14ac:dyDescent="0.25">
@@ -1241,7 +1497,7 @@
         <v>2</v>
       </c>
       <c r="M45" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="9:13" x14ac:dyDescent="0.25">
@@ -1273,24 +1529,1517 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <f>A1-A2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>A2-A3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>A3-A4</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>A4-A5</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-6</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>A5-A6</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>D8/9</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>E8*100</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E53" si="0">D9/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F53" si="1">E9*100</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="G9">
+        <v>0.26190476000000001</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="G10">
+        <v>0.52380952000000003</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="G11">
+        <v>0.78571427999999999</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>44.444444444444443</v>
+      </c>
+      <c r="G12">
+        <v>1.0476190400000001</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="G13">
+        <v>1.3095238</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f>(30-8)/9-13/100</f>
+        <v>2.3144444444444447</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="G14">
+        <v>1.57142856</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <f>(30-8)/9-2/100</f>
+        <v>2.4244444444444446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>77.777777777777786</v>
+      </c>
+      <c r="G15">
+        <v>1.8333333199999999</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <f>(30-8)/9-14/100</f>
+        <v>2.3044444444444445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="G16">
+        <v>2.0952380800000001</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G17">
+        <v>2.3571428399999999</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>111.11111111111111</v>
+      </c>
+      <c r="G18">
+        <v>2.6190476</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.2222222222222223</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>122.22222222222223</v>
+      </c>
+      <c r="G19">
+        <v>2.8809523600000002</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>133.33333333333331</v>
+      </c>
+      <c r="G20">
+        <v>3.1428571199999999</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>13</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>144.44444444444443</v>
+      </c>
+      <c r="G21">
+        <v>3.4047618800000001</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1.5555555555555556</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>155.55555555555557</v>
+      </c>
+      <c r="G22">
+        <v>3.6666666399999999</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>166.66666666666669</v>
+      </c>
+      <c r="G23">
+        <v>3.9285714</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1.7777777777777777</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>177.77777777777777</v>
+      </c>
+      <c r="G24">
+        <v>4.1904761600000002</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>17</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.8888888888888888</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>188.88888888888889</v>
+      </c>
+      <c r="G25">
+        <v>4.4523809200000004</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>18</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="G26">
+        <v>4.7142856799999997</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>19</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2.1111111111111112</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>211.11111111111111</v>
+      </c>
+      <c r="G27">
+        <v>4.9761904399999999</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>20</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>222.22222222222223</v>
+      </c>
+      <c r="G28">
+        <v>5.2380952000000001</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>233.33333333333334</v>
+      </c>
+      <c r="G29">
+        <v>5.4999999600000002</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>22</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>2.4444444444444446</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>244.44444444444446</v>
+      </c>
+      <c r="G30">
+        <v>5.7619047200000004</v>
+      </c>
+      <c r="I30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>23</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>2.5555555555555554</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>255.55555555555554</v>
+      </c>
+      <c r="G31">
+        <v>6.0238094799999997</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>24</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>266.66666666666663</v>
+      </c>
+      <c r="G32">
+        <v>6.2857142399999999</v>
+      </c>
+      <c r="I32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>25</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>277.77777777777777</v>
+      </c>
+      <c r="G33">
+        <v>6.5476190000000001</v>
+      </c>
+      <c r="I33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>2.8888888888888888</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>288.88888888888886</v>
+      </c>
+      <c r="G34">
+        <v>6.8095237600000003</v>
+      </c>
+      <c r="I34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>27</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="G35">
+        <v>7.0714285200000004</v>
+      </c>
+      <c r="H35">
+        <v>7</v>
+      </c>
+      <c r="I35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>311.11111111111114</v>
+      </c>
+      <c r="G36">
+        <v>7.3333332799999997</v>
+      </c>
+      <c r="I36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>29</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>3.2222222222222223</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>322.22222222222223</v>
+      </c>
+      <c r="G37">
+        <v>7.5952380399999999</v>
+      </c>
+      <c r="I37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>30</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>333.33333333333337</v>
+      </c>
+      <c r="G38">
+        <v>7.8571428000000001</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>-1</v>
+      </c>
+      <c r="D39">
+        <v>31</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>3.4444444444444446</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>344.44444444444446</v>
+      </c>
+      <c r="G39">
+        <v>8.1190475600000003</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>-2</v>
+      </c>
+      <c r="D40">
+        <v>32</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>3.5555555555555554</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>355.55555555555554</v>
+      </c>
+      <c r="G40">
+        <v>8.3809523200000005</v>
+      </c>
+      <c r="I40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>-3</v>
+      </c>
+      <c r="D41">
+        <v>33</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>366.66666666666663</v>
+      </c>
+      <c r="G41">
+        <v>8.6428570800000006</v>
+      </c>
+      <c r="I41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>-4</v>
+      </c>
+      <c r="D42">
+        <v>34</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>3.7777777777777777</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>377.77777777777777</v>
+      </c>
+      <c r="G42">
+        <v>8.9047618400000008</v>
+      </c>
+      <c r="I42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>-5</v>
+      </c>
+      <c r="D43">
+        <v>35</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>3.8888888888888888</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>388.88888888888886</v>
+      </c>
+      <c r="G43">
+        <v>9.1666665999999992</v>
+      </c>
+      <c r="H43">
+        <v>9</v>
+      </c>
+      <c r="I43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>-6</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>36</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="G44">
+        <v>9.4285713599999994</v>
+      </c>
+      <c r="I44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>-7</v>
+      </c>
+      <c r="D45">
+        <v>37</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>4.1111111111111107</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>411.11111111111109</v>
+      </c>
+      <c r="G45">
+        <v>9.6904761199999996</v>
+      </c>
+      <c r="I45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>-8</v>
+      </c>
+      <c r="D46">
+        <v>38</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>4.2222222222222223</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>422.22222222222223</v>
+      </c>
+      <c r="G46">
+        <v>9.9523808799999998</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>-9</v>
+      </c>
+      <c r="D47">
+        <v>39</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>433.33333333333331</v>
+      </c>
+      <c r="G47">
+        <v>10.21428564</v>
+      </c>
+      <c r="H47">
+        <v>10</v>
+      </c>
+      <c r="I47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>-10</v>
+      </c>
+      <c r="D48">
+        <v>40</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>444.44444444444446</v>
+      </c>
+      <c r="G48">
+        <v>10.4761904</v>
+      </c>
+      <c r="I48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>-11</v>
+      </c>
+      <c r="D49">
+        <v>41</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>4.5555555555555554</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>455.55555555555554</v>
+      </c>
+      <c r="G49">
+        <v>10.73809516</v>
+      </c>
+      <c r="I49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>-12</v>
+      </c>
+      <c r="D50">
+        <v>42</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>466.66666666666669</v>
+      </c>
+      <c r="G50">
+        <v>10.99999992</v>
+      </c>
+      <c r="H50">
+        <v>11</v>
+      </c>
+      <c r="I50">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>-13</v>
+      </c>
+      <c r="D51">
+        <v>43</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>4.7777777777777777</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>477.77777777777777</v>
+      </c>
+      <c r="G51">
+        <v>11.261904680000001</v>
+      </c>
+      <c r="I51">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>-14</v>
+      </c>
+      <c r="D52">
+        <v>44</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>4.8888888888888893</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>488.88888888888891</v>
+      </c>
+      <c r="G52">
+        <v>11.523809440000001</v>
+      </c>
+      <c r="I52">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>-15</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>45</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="G53">
+        <v>11.785714199999999</v>
+      </c>
+      <c r="I53">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
+        <v>0.3</v>
+      </c>
+      <c r="F4">
+        <v>0.4</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>0.6</v>
+      </c>
+      <c r="I4">
+        <v>0.7</v>
+      </c>
+      <c r="J4">
+        <v>0.8</v>
+      </c>
+      <c r="K4">
+        <v>0.9</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N4">
+        <v>1.2</v>
+      </c>
+      <c r="O4">
+        <v>1.3</v>
+      </c>
+      <c r="P4">
+        <v>1.4</v>
+      </c>
+      <c r="Q4">
+        <v>1.5</v>
+      </c>
+      <c r="R4">
+        <v>1.6</v>
+      </c>
+      <c r="S4">
+        <v>1.7</v>
+      </c>
+      <c r="T4">
+        <v>1.8</v>
+      </c>
+      <c r="U4">
+        <v>1.9</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" s="11">
+        <v>-9.2799999999999994</v>
+      </c>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6" s="11">
+        <v>-8.75</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" s="11">
+        <v>-8.2200000000000006</v>
+      </c>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11">
+        <v>-7.69</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9" s="11">
+        <v>-7.16</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>15</v>
+      </c>
+      <c r="B10" s="11">
+        <v>-6.63</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" s="12">
+        <v>-6.1</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12" s="12">
+        <v>-5.5699999999999994</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13" s="12">
+        <v>-5.0399999999999991</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>19</v>
+      </c>
+      <c r="B14" s="12">
+        <v>-4.5099999999999989</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" s="12">
+        <v>-3.9799999999999986</v>
+      </c>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>21</v>
+      </c>
+      <c r="B16" s="12">
+        <v>-3.4499999999999984</v>
+      </c>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" s="12">
+        <v>-2.9199999999999982</v>
+      </c>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>23</v>
+      </c>
+      <c r="B18" s="12">
+        <v>-2.3899999999999979</v>
+      </c>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>24</v>
+      </c>
+      <c r="B19" s="12">
+        <v>-1.8599999999999979</v>
+      </c>
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>25</v>
+      </c>
+      <c r="B20" s="12">
+        <v>-1.3299999999999979</v>
+      </c>
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>26</v>
+      </c>
+      <c r="B21" s="12">
+        <v>-0.79999999999999782</v>
+      </c>
+      <c r="C21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>27</v>
+      </c>
+      <c r="B22" s="12">
+        <v>-0.2699999999999978</v>
+      </c>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>28</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.26000000000000223</v>
+      </c>
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>29</v>
+      </c>
+      <c r="B24" s="12">
+        <v>0.79000000000000226</v>
+      </c>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>30</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1.3200000000000023</v>
+      </c>
+      <c r="C25" s="12">
+        <v>1.47</v>
+      </c>
+      <c r="D25">
+        <v>1.58</v>
+      </c>
+      <c r="E25">
+        <v>1.67</v>
+      </c>
+      <c r="F25">
+        <v>1.74</v>
+      </c>
+      <c r="G25">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="45" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>2</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>4</v>
+      </c>
+      <c r="M45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="L48">
+        <v>4</v>
+      </c>
+      <c r="M48">
+        <v>5</v>
+      </c>
+      <c r="N48">
+        <v>6</v>
+      </c>
+      <c r="O48">
+        <v>7</v>
+      </c>
+      <c r="P48">
+        <v>8</v>
+      </c>
+      <c r="Q48">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DBField added, app was tested, all works fine
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="23280" windowHeight="12990"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="23280" windowHeight="12990" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>Количество верхней одежды</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t>tem\clo</t>
+  </si>
+  <si>
+    <t>Температура</t>
+  </si>
+  <si>
+    <t>Количество слойев</t>
+  </si>
+  <si>
+    <t>Сумма индексов</t>
+  </si>
+  <si>
+    <t>Средний индекс</t>
   </si>
 </sst>
 </file>
@@ -571,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3042,4 +3054,940 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>E2/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D42" si="0">C3/B3</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F42" si="1">E3/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>7.333333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>7.666666666666667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="E27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="E28">
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>9.3333333333333339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>29</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>9.6666666666666661</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E32">
+        <v>31</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>10.333333333333334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-1</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E33">
+        <v>32</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-2</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E34">
+        <v>33</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-3</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E35">
+        <v>34</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>11.333333333333334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>-4</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="E36">
+        <v>35</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>11.666666666666666</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>-5</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="E37">
+        <v>36</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>-6</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>11</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="E38">
+        <v>37</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>-7</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>38</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>12.666666666666666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>-8</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>12</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>39</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>-9</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>12</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>40</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>-10</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>12</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>41</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>13.666666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
boots was added, click listener on LooksActivity
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>Количество верхней одежды</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>Средний индекс</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>layers</t>
+  </si>
+  <si>
+    <t>temp</t>
   </si>
 </sst>
 </file>
@@ -254,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -262,11 +274,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -280,6 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3058,10 +3080,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,7 +3093,7 @@
     <col min="3" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -3085,7 +3107,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>33</v>
       </c>
@@ -3099,8 +3126,14 @@
         <f t="shared" ref="F3:F26" si="0">E3/(4*B3)</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>32</v>
       </c>
@@ -3114,8 +3147,21 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4">
+        <f>A3</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>31</v>
       </c>
@@ -3129,8 +3175,20 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>30</v>
       </c>
@@ -3151,8 +3209,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>29</v>
       </c>
@@ -3173,8 +3243,14 @@
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>28</v>
       </c>
@@ -3195,8 +3271,14 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27</v>
       </c>
@@ -3217,8 +3299,14 @@
         <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>26</v>
       </c>
@@ -3239,8 +3327,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>25</v>
       </c>
@@ -3261,8 +3355,14 @@
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>24</v>
       </c>
@@ -3283,8 +3383,14 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23</v>
       </c>
@@ -3305,30 +3411,42 @@
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>22</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E14">
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E14" s="13">
         <v>12</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G14" s="13">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>21</v>
       </c>
@@ -3349,8 +3467,18 @@
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <f>G15*2</f>
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20</v>
       </c>
@@ -3368,11 +3496,21 @@
         <v>14</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f>E16/(4*B16)</f>
         <v>1.75</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <f>G16*2</f>
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>19</v>
       </c>
@@ -3393,8 +3531,18 @@
         <f t="shared" si="0"/>
         <v>1.875</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <f>G17*2</f>
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -3415,8 +3563,18 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H29" si="2">G18*2</f>
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3437,8 +3595,18 @@
         <f t="shared" si="0"/>
         <v>2.125</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3459,8 +3627,18 @@
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -3481,8 +3659,18 @@
         <f t="shared" si="0"/>
         <v>2.375</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
@@ -3503,8 +3691,18 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>13</v>
       </c>
@@ -3525,8 +3723,18 @@
         <f t="shared" si="0"/>
         <v>2.625</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -3547,8 +3755,18 @@
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
@@ -3569,8 +3787,18 @@
         <f t="shared" si="0"/>
         <v>2.875</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10</v>
       </c>
@@ -3591,8 +3819,18 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -3613,8 +3851,18 @@
         <f>E27/(4*B27)</f>
         <v>3.125</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8</v>
       </c>
@@ -3632,33 +3880,53 @@
         <v>26</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F4:F46" si="2">E28/(3.5*B28)</f>
+        <f t="shared" ref="F28:F46" si="3">E28/(3.5*B28)</f>
         <v>2.4761904761904763</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
         <v>7</v>
       </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="13">
+        <v>3</v>
+      </c>
+      <c r="C29" s="13">
         <v>8</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="13">
         <f t="shared" si="1"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="13">
         <v>27</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="13">
+        <f t="shared" si="3"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="G29" s="13">
+        <v>6</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="2"/>
-        <v>2.5714285714285716</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -3676,11 +3944,21 @@
         <v>28</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.6666666666666665</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <f>G30*3</f>
+        <v>9</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -3698,11 +3976,21 @@
         <v>29</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7619047619047619</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:H50" si="4">G31*3</f>
+        <v>9</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3720,11 +4008,21 @@
         <v>30</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.8571428571428572</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -3742,11 +4040,21 @@
         <v>31</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9523809523809526</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -3764,11 +4072,21 @@
         <v>32</v>
       </c>
       <c r="F34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0476190476190474</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -3786,11 +4104,21 @@
         <v>33</v>
       </c>
       <c r="F35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1428571428571428</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -3808,11 +4136,21 @@
         <v>34</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.2380952380952381</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>-1</v>
       </c>
@@ -3830,11 +4168,21 @@
         <v>35</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3333333333333335</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-2</v>
       </c>
@@ -3852,11 +4200,21 @@
         <v>36</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.4285714285714284</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-3</v>
       </c>
@@ -3874,11 +4232,21 @@
         <v>37</v>
       </c>
       <c r="F39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5238095238095237</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-4</v>
       </c>
@@ -3896,11 +4264,21 @@
         <v>38</v>
       </c>
       <c r="F40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.6190476190476191</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-5</v>
       </c>
@@ -3918,11 +4296,21 @@
         <v>39</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7142857142857144</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>6</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-6</v>
       </c>
@@ -3940,11 +4328,21 @@
         <v>40</v>
       </c>
       <c r="F42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.8095238095238093</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>7</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-7</v>
       </c>
@@ -3962,11 +4360,21 @@
         <v>41</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.9047619047619047</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>7</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-8</v>
       </c>
@@ -3984,11 +4392,21 @@
         <v>42</v>
       </c>
       <c r="F44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>7</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-9</v>
       </c>
@@ -4006,11 +4424,21 @@
         <v>43</v>
       </c>
       <c r="F45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.0952380952380949</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>8</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-10</v>
       </c>
@@ -4028,8 +4456,63 @@
         <v>44</v>
       </c>
       <c r="F46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.1904761904761907</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>-11</v>
+      </c>
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>-12</v>
+      </c>
+      <c r="G48">
+        <v>9</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>-13</v>
+      </c>
+      <c r="G49">
+        <v>9</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>-14</v>
+      </c>
+      <c r="G50">
+        <v>9</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="4"/>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>